<commit_message>
Thêm nhân viên bằng excel
</commit_message>
<xml_diff>
--- a/phim2101/Upload/test.xlsx
+++ b/phim2101/Upload/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387910E4-930B-4DC2-ABA4-74C3260ACDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB82F15C-C0EF-4769-A2C6-463249760065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17841029-9D10-473A-95BF-951F66BE6EA6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>MaPhim</t>
   </si>
@@ -90,32 +90,26 @@
     <t>Âu Mỹ</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=zxXlm0fguHU&amp;t=11s</t>
-  </si>
-  <si>
-    <t>https://chieuphimquocgia.com.vn/Content/Images/0016616_0.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Một bộ phim hài phiêu lưu theo chân một ca sĩ nổi tiếng một thời trở về quê hương và tham gia một cuộc thi khoan giếng nước với hy vọng giành được một giải thưởng tiền mặt lớn. Nhưng những gì họ không nhận ra là một con thú bí ẩn ẩn nấp dưới lòng đất.</t>
-  </si>
-  <si>
     <t>144p</t>
   </si>
   <si>
-    <t>09-12-2022  20:20:00 PM</t>
-  </si>
-  <si>
-    <t>09-12-2022  22:20:00 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ahihitesst </t>
+    <t>ahihitesst</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gPMaf2aw0xM</t>
+  </si>
+  <si>
+    <t>/Images/fast.png</t>
+  </si>
+  <si>
+    <t>Một bộ phim hài phiêu lưu theo chân một ca sĩ nổi tiếng một thời trở về quê hương và tham gia một cuộc thi khoan giếng nước với hy vọng giành được một giải thưởng tiền mặt lớn. Nhưng những gì họ không nhận ra là một con thú bí ẩn ẩn nấp dưới lòng đất.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,11 +133,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -175,9 +164,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,10 +487,14 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -544,7 +539,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -577,41 +572,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1">
+    <row r="3" spans="1:12" ht="138" customHeight="1">
+      <c r="A3" s="5">
         <v>23</v>
       </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="5">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="J3" s="6">
+        <v>44904.847222222219</v>
+      </c>
+      <c r="K3" s="6">
+        <v>44904.930555555555</v>
+      </c>
+      <c r="L3" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test chức năng mua vé không trùng (chưa xong)
</commit_message>
<xml_diff>
--- a/phim2101/Upload/test.xlsx
+++ b/phim2101/Upload/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB82F15C-C0EF-4769-A2C6-463249760065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28C4DAB-33A9-4B5A-B251-31677E3292E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17841029-9D10-473A-95BF-951F66BE6EA6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>MaPhim</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Úc</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=bYqOE75XBMQ&amp;t=2s</t>
-  </si>
-  <si>
-    <t>https://img.ophim.cc/uploads/movies/giai-cuu-cay-uoc-nguyen-thumb.jpg</t>
-  </si>
-  <si>
     <t>Giải Cứu Cây Ước Nguyện The Wishmas Tree Bộ phim hoạt hình của Úc nói về Mong ước sai lầm của một chú chuột túi trẻ về một Wishmas màu trắng không chỉ đóng băng toàn bộ thành phố Sanctuary thành phố quê hương của cô mà còn đe dọa cuộc sống của tất cả những người sống ở đó. Trước khi Cây Wishmas ma thuật chết đi, cô ấy phải thực hiện một cuộc hành trình đầy nguy hiểm vào WILD; chiến đấu với sự nghi ngờ bản thân, những kẻ săn mồi ma quái và cuối cùng là Sự tuyệt chủng để đảo ngược những thiệt hại mà cô đã gây ra và cứu thành phố của mình.</t>
   </si>
   <si>
@@ -87,22 +81,46 @@
     <t>08-12-2022  21:30:00 PM</t>
   </si>
   <si>
-    <t>Âu Mỹ</t>
-  </si>
-  <si>
     <t>144p</t>
   </si>
   <si>
-    <t>ahihitesst</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=gPMaf2aw0xM</t>
-  </si>
-  <si>
-    <t>/Images/fast.png</t>
-  </si>
-  <si>
-    <t>Một bộ phim hài phiêu lưu theo chân một ca sĩ nổi tiếng một thời trở về quê hương và tham gia một cuộc thi khoan giếng nước với hy vọng giành được một giải thưởng tiền mặt lớn. Nhưng những gì họ không nhận ra là một con thú bí ẩn ẩn nấp dưới lòng đất.</t>
+    <t>Kẻ độc hành</t>
+  </si>
+  <si>
+    <t>Việt Nam</t>
+  </si>
+  <si>
+    <t>Mỹ</t>
+  </si>
+  <si>
+    <t>Black Adam</t>
+  </si>
+  <si>
+    <t>125 phút</t>
+  </si>
+  <si>
+    <t>Black Adam là một bộ phim điện ảnh siêu anh hùng của Hoa Kỳ ra mắt năm 2022, dựa trên nhân vật cùng tên của DC Comics. Được sản xuất bởi New Line Cinema, DC Films, Seven Bucks Productions và Flynn Picture, đây là phần phim ngoại truyện của Shazam! (2019), và là phim thứ 11 trong Vũ trụ Mở rộng DC (DCEU). Được đạo diễn bởi Jaume Collet-Serra và được viết kịch bản bởi Adam Sztykiel, Rory Haines và Sohrab Noshirvani, bộ phim có sự tham gia của Dwayne Johnson trong vai nhân vật chính cùng với Aldis Hodge, Noah Centineo, Sarah Shahi, Marwan Kenzari, Quintessa Swindell, Bodhi Sabongui và Pierce Brosnan.</t>
+  </si>
+  <si>
+    <t>/Images/adam.jpg</t>
+  </si>
+  <si>
+    <t>/Images/kedochanh.jpg</t>
+  </si>
+  <si>
+    <t>/Images/nhims.jpg</t>
+  </si>
+  <si>
+    <t>Kẻ Độc Hành là mảnh ghép đặc biệt của web-drama Ai Chết Giơ Tay và phim điện ảnh Pháp Sư Mù mà Huỳnh Lập từng thực hiện. Phim bật mí cho khán giả những câu chuyện bi hài về thân thế của nhân vật Tinh Lâm, trước khi anh trở thành pháp sư trong Ai Chết Giơ Tay. Phần tiền truyện này xoay quanh cuộc sống của chàng trai trẻ Tinh Lâm (Huỳnh Lập) làm nghề bán vòng phong thủy và có niềm đam mê mãnh liệt với thế giới tâm linh. Cha mẹ anh mất sớm nên gia đình chỉ còn lại ông Vú (Quốc Khánh) để anh nương tựa và chăm sóc.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/mkomfZHG5q4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/_iyC2aUCxY0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/bYqOE75XBMQ&amp;t=2s</t>
   </si>
 </sst>
 </file>
@@ -124,16 +142,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color indexed="30"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,25 +172,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,16 +509,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E86C4E7-0BB5-448E-A9E8-58FE51F8682A}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -536,7 +560,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>8</v>
@@ -548,71 +572,113 @@
         <v>13</v>
       </c>
       <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="L2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="138" customHeight="1">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" ht="18" customHeight="1">
+      <c r="A3" s="4">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="7">
+        <v>44925.847222222219</v>
+      </c>
+      <c r="K3" s="7">
+        <v>44925.930555555555</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="6">
-        <v>44904.847222222219</v>
-      </c>
-      <c r="K3" s="6">
-        <v>44904.930555555555</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="J4" s="7">
+        <v>44925.847222222219</v>
+      </c>
+      <c r="K4" s="7">
+        <v>44925.930555555555</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="https://www.youtube.com/watch?v=bYqOE75XBMQ&amp;t=2s" xr:uid="{6DA394D5-FBDA-4CF5-AF70-13C1D7D50089}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6DA394D5-FBDA-4CF5-AF70-13C1D7D50089}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{F3D0F8A1-D1DE-4A63-A79E-46378237F4F6}"/>
+    <hyperlink ref="G3" r:id="rId3" display="https://thegioidienanh.vn/stores/news_dataimages/hath/102022/20/11/2154_PAYOFF_THE_YOUNG_SHAMAN.jpg?rt=20221020112206" xr:uid="{3788759D-74F2-40BA-86F5-93CFD334AF73}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{82F97094-4F52-41E5-AC78-87044C085604}"/>
+    <hyperlink ref="G4" r:id="rId5" display="https://encrypted-tbn2.gstatic.com/images?q=tbn:ANd9GcTHeMjDbZjNkZZHJhAbB72UVmQEhtAf0X6bAi_ouN-pbUvLOIfH" xr:uid="{7DD15A10-B628-43BB-8C4C-09D9E0642E4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>